<commit_message>
IV; fix NAs in control_variables and re-export corresponding tables
</commit_message>
<xml_diff>
--- a/xlsx/country_comparison/gcs_support_by_variant_warm_glow.xlsx
+++ b/xlsx/country_comparison/gcs_support_by_variant_warm_glow.xlsx
@@ -416,13 +416,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0345677812512016</v>
+        <v>0.027657737928523</v>
       </c>
       <c r="C2" t="n">
-        <v>0.00955330665890686</v>
+        <v>0.00393672748029645</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0595822558434964</v>
+        <v>0.0513787483767496</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -433,13 +433,13 @@
         <v>7</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0675876450707566</v>
+        <v>0.0537545332660761</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0333189915956314</v>
+        <v>0.0208975824207113</v>
       </c>
       <c r="D3" t="n">
-        <v>0.101856298545882</v>
+        <v>0.0866114841114409</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
@@ -450,13 +450,13 @@
         <v>8</v>
       </c>
       <c r="B4" t="n">
-        <v>0.0391366742932622</v>
+        <v>0.0484519454118784</v>
       </c>
       <c r="C4" t="n">
-        <v>-0.042578009691438</v>
+        <v>-0.0311976696309093</v>
       </c>
       <c r="D4" t="n">
-        <v>0.120851358277962</v>
+        <v>0.128101560454666</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>
@@ -467,13 +467,13 @@
         <v>9</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0947531111645335</v>
+        <v>0.0871006762458434</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0191488053021976</v>
+        <v>0.0139036353963154</v>
       </c>
       <c r="D5" t="n">
-        <v>0.170357417026869</v>
+        <v>0.160297717095371</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
@@ -484,13 +484,13 @@
         <v>10</v>
       </c>
       <c r="B6" t="n">
-        <v>0.0175119326214762</v>
+        <v>0.0173450096068929</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.0577422545335324</v>
+        <v>-0.058688821276682</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0927661197764848</v>
+        <v>0.0933788404904679</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -501,13 +501,13 @@
         <v>11</v>
       </c>
       <c r="B7" t="n">
-        <v>0.103853982432025</v>
+        <v>0.0996831072386706</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.00231517261693412</v>
+        <v>-0.00856427756722054</v>
       </c>
       <c r="D7" t="n">
-        <v>0.210023137480985</v>
+        <v>0.207930492044562</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
@@ -518,13 +518,13 @@
         <v>12</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0456890966545247</v>
+        <v>0.0283852722219771</v>
       </c>
       <c r="C8" t="n">
-        <v>-0.0503919462261996</v>
+        <v>-0.0667645085984285</v>
       </c>
       <c r="D8" t="n">
-        <v>0.141770139535249</v>
+        <v>0.123535053042383</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
@@ -535,13 +535,13 @@
         <v>13</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0834478409431803</v>
+        <v>0.0534873354293704</v>
       </c>
       <c r="C9" t="n">
-        <v>-0.000972477118733037</v>
+        <v>-0.0253330284234113</v>
       </c>
       <c r="D9" t="n">
-        <v>0.167868159005094</v>
+        <v>0.132307699282152</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
@@ -552,13 +552,13 @@
         <v>14</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0490455807248947</v>
+        <v>0.0535469667124348</v>
       </c>
       <c r="C10" t="n">
-        <v>-0.0594078178313194</v>
+        <v>-0.0550456393798702</v>
       </c>
       <c r="D10" t="n">
-        <v>0.157498979281109</v>
+        <v>0.16213957280474</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
@@ -569,13 +569,13 @@
         <v>15</v>
       </c>
       <c r="B11" t="n">
-        <v>0.0101133748194984</v>
+        <v>0.00806816490614442</v>
       </c>
       <c r="C11" t="n">
-        <v>-0.0428318682783557</v>
+        <v>-0.0449560745181978</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0630586179173526</v>
+        <v>0.0610924043304867</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
@@ -586,13 +586,13 @@
         <v>16</v>
       </c>
       <c r="B12" t="n">
-        <v>0.00777904174477409</v>
+        <v>0.000561717691077912</v>
       </c>
       <c r="C12" t="n">
-        <v>-0.0365787724650717</v>
+        <v>-0.0410132178650919</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0521368559546199</v>
+        <v>0.0421366532472477</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>

</xml_diff>